<commit_message>
integrated into a database using sqlite3
</commit_message>
<xml_diff>
--- a/datasets/unlisted_df.xlsx
+++ b/datasets/unlisted_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\PycharmProjects\Scrapy\Unlisted-Zone-Shares\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52A8FFC-2C13-4AD4-A637-0F684E1EC2E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BD935B-02D0-4C2F-8037-066B46BEA370}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1843,13 +1843,13 @@
   <dimension ref="A1:E243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="70" customWidth="1"/>
-    <col min="3" max="5" width="31" customWidth="1"/>
+    <col min="2" max="2" width="75" customWidth="1"/>
+    <col min="3" max="5" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>